<commit_message>
First commit of the framework
</commit_message>
<xml_diff>
--- a/TestData/Preprod.xlsx
+++ b/TestData/Preprod.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diksha_sel\Diksha_Prepod\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6438A673-7F2A-4926-80C6-4F3BCC2B59E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6438A673-7F2A-4926-80C6-4F3BCC2B59E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA217669-9719-45FE-93B1-165B63F85D57}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="TestData" sheetId="5" r:id="rId2"/>
     <sheet name="Course" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="356">
+  <si>
+    <t>Role</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
@@ -43,348 +46,372 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>ContentCreatortn@yopmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>contentreviewertn@yopmail.com</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>mentorsun@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Orgadminsun@gmail.com</t>
+  </si>
+  <si>
+    <t>Public User1</t>
+  </si>
+  <si>
+    <t>usersun@gmail.com</t>
+  </si>
+  <si>
+    <t>Public User2</t>
+  </si>
+  <si>
+    <t>Book Creator</t>
+  </si>
+  <si>
+    <t>suborgcreatorsun@gmail.com</t>
+  </si>
+  <si>
+    <t>Book Reviewer</t>
+  </si>
+  <si>
+    <t>suborgreviewersun@gmail.com</t>
+  </si>
+  <si>
+    <t>Mentor2</t>
+  </si>
+  <si>
+    <t>tncontentcreator@yopmail.com</t>
+  </si>
+  <si>
+    <t>Creator2</t>
+  </si>
+  <si>
+    <t>TCTestUser</t>
+  </si>
+  <si>
+    <t>automation123@yopmail.com</t>
+  </si>
+  <si>
+    <t>FrameworkUser</t>
+  </si>
+  <si>
+    <t>tejas.teju110@gmail.com</t>
+  </si>
+  <si>
+    <t>NewUserSecondTime</t>
+  </si>
+  <si>
+    <t>secondtimeuser@yopmail.com</t>
+  </si>
+  <si>
+    <t>UnAuthenticUser</t>
+  </si>
+  <si>
+    <t>suborgdiffadmin@yopmail.com</t>
+  </si>
+  <si>
+    <t>SubOrgMentor</t>
+  </si>
+  <si>
+    <t>suborgdiffcoursementor@yopmail.com</t>
+  </si>
+  <si>
+    <t>SubOrgMentor2</t>
+  </si>
+  <si>
+    <t>suborgmentorsun@gmail.com</t>
+  </si>
+  <si>
+    <t>CustodianUser</t>
+  </si>
+  <si>
+    <t>preproduser@yopmail.com</t>
+  </si>
+  <si>
+    <t>StateTenant</t>
+  </si>
+  <si>
+    <t>suborgdiffbookcreator@yopmail.com</t>
+  </si>
+  <si>
+    <t>SubOrgReviewer</t>
+  </si>
+  <si>
+    <t>suborgdiffcontentreviewer@yopmail.com</t>
+  </si>
+  <si>
+    <t>CreatorRJ</t>
+  </si>
+  <si>
+    <t>contentcreatorRJ@yopmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>Admin4</t>
+  </si>
+  <si>
+    <t>portalpreprod30@yopmail.com</t>
+  </si>
+  <si>
+    <t>Custod2</t>
+  </si>
+  <si>
+    <t>custod2user@yopmail.com</t>
+  </si>
+  <si>
+    <t>Admin3</t>
+  </si>
+  <si>
+    <t>demoorgadmin@tn.com</t>
+  </si>
+  <si>
+    <t>demo123</t>
+  </si>
+  <si>
+    <t>InvalidUser</t>
+  </si>
+  <si>
+    <t>InvalidUser@yopmail.com</t>
+  </si>
+  <si>
+    <t>Custodian3</t>
+  </si>
+  <si>
+    <t>custodian993@yopmail.com</t>
+  </si>
+  <si>
+    <t>ContentCreator</t>
+  </si>
+  <si>
+    <t>NoBoard</t>
+  </si>
+  <si>
+    <t>bcontentcreator@yopmail.com</t>
+  </si>
+  <si>
+    <t>ContentReviewer</t>
+  </si>
+  <si>
+    <t>contentreviewerTN@yopmail.com</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>pnr15@yopmail.com</t>
+  </si>
+  <si>
+    <t>MinorUser</t>
+  </si>
+  <si>
+    <t>childuser@yopmail.com</t>
+  </si>
+  <si>
+    <t>NCERTCC</t>
+  </si>
+  <si>
+    <t>ncertcontentcreator100@yopmail.com</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>NCERTCR</t>
+  </si>
+  <si>
+    <t>ncertcontentreviewer100@yopmail.com</t>
+  </si>
+  <si>
+    <t>NewCustUser</t>
+  </si>
+  <si>
+    <t>preprod40@yopmail.com</t>
+  </si>
+  <si>
+    <t>VerifyMembers</t>
+  </si>
+  <si>
+    <t>stag58@yopmail.com</t>
+  </si>
+  <si>
+    <t>DeleteGroup1</t>
+  </si>
+  <si>
+    <t>preprod38@yopmail.com</t>
+  </si>
+  <si>
+    <t>deleteMember1</t>
+  </si>
+  <si>
+    <t>group19@yopmail.com</t>
+  </si>
+  <si>
+    <t>Tntenant</t>
+  </si>
+  <si>
+    <t>Tnorgadmin@yopmail.com</t>
+  </si>
+  <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>APTenantCreator</t>
+  </si>
+  <si>
+    <t>apcontentcreator100@yopmail.com</t>
+  </si>
+  <si>
+    <t>apcontentreviewer100@yopmail.com</t>
+  </si>
+  <si>
+    <t>NewCredCourseToc</t>
+  </si>
+  <si>
+    <t>stag55@yopmail.com</t>
+  </si>
+  <si>
+    <t>Dont Use</t>
+  </si>
+  <si>
+    <t>stagdu@yopmail.com</t>
+  </si>
+  <si>
+    <t>No Groups</t>
+  </si>
+  <si>
+    <t>stagn@yopmail.com</t>
+  </si>
+  <si>
+    <t>Group Member</t>
+  </si>
+  <si>
+    <t>userv1@yopmail.com</t>
+  </si>
+  <si>
+    <t>AddUserCred</t>
+  </si>
+  <si>
+    <t>adduserswitch1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>preprod50@yopmail.com</t>
+  </si>
+  <si>
+    <t>submitDetails</t>
+  </si>
+  <si>
+    <t>submitdetailsprofpage@yopmail.com</t>
+  </si>
+  <si>
+    <t>memberaddedgroup</t>
+  </si>
+  <si>
+    <t>memberaddedgroup@yopmail.com</t>
+  </si>
+  <si>
+    <t>MobileNumberRegistedUser</t>
+  </si>
+  <si>
+    <t>certficateTabValidation</t>
+  </si>
+  <si>
+    <t>userdd@yopmail.com</t>
+  </si>
+  <si>
+    <t>ContentCreator1</t>
+  </si>
+  <si>
+    <t>globe1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Pass@123</t>
+  </si>
+  <si>
+    <t>globe</t>
+  </si>
+  <si>
+    <t>OrgAdmin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>submitProfile</t>
+  </si>
+  <si>
+    <t>OnlyCreator</t>
+  </si>
+  <si>
+    <t>Content Type</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>do_id</t>
+  </si>
+  <si>
+    <t>TitleDescription</t>
+  </si>
+  <si>
+    <t>CourseDescription</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>frGdlx</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CourseName</t>
+  </si>
+  <si>
     <t>Execute Test?</t>
   </si>
   <si>
+    <t>CourseA</t>
+  </si>
+  <si>
+    <t>CourseA Description</t>
+  </si>
+  <si>
+    <t>CourseA Title</t>
+  </si>
+  <si>
+    <t>CourseA Title Description</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Creator</t>
-  </si>
-  <si>
-    <t>ContentCreatortn@yopmail.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Reviewer</t>
-  </si>
-  <si>
-    <t>contentreviewertn@yopmail.com</t>
-  </si>
-  <si>
-    <t>Mentor</t>
-  </si>
-  <si>
-    <t>mentorsun@gmail.com</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Orgadminsun@gmail.com</t>
-  </si>
-  <si>
-    <t>Public User1</t>
-  </si>
-  <si>
-    <t>usersun@gmail.com</t>
-  </si>
-  <si>
-    <t>Public User2</t>
-  </si>
-  <si>
-    <t>Book Creator</t>
-  </si>
-  <si>
-    <t>suborgcreatorsun@gmail.com</t>
-  </si>
-  <si>
-    <t>Book Reviewer</t>
-  </si>
-  <si>
-    <t>suborgreviewersun@gmail.com</t>
-  </si>
-  <si>
-    <t>Mentor2</t>
-  </si>
-  <si>
-    <t>tncontentcreator@yopmail.com</t>
-  </si>
-  <si>
-    <t>Creator2</t>
-  </si>
-  <si>
-    <t>TCTestUser</t>
-  </si>
-  <si>
-    <t>automation123@yopmail.com</t>
-  </si>
-  <si>
-    <t>FrameworkUser</t>
-  </si>
-  <si>
-    <t>tejas.teju110@gmail.com</t>
-  </si>
-  <si>
-    <t>NewUserSecondTime</t>
-  </si>
-  <si>
-    <t>secondtimeuser@yopmail.com</t>
-  </si>
-  <si>
-    <t>UnAuthenticUser</t>
-  </si>
-  <si>
-    <t>suborgdiffadmin@yopmail.com</t>
-  </si>
-  <si>
-    <t>SubOrgMentor</t>
-  </si>
-  <si>
-    <t>suborgdiffcoursementor@yopmail.com</t>
-  </si>
-  <si>
-    <t>SubOrgMentor2</t>
-  </si>
-  <si>
-    <t>suborgmentorsun@gmail.com</t>
-  </si>
-  <si>
-    <t>CustodianUser</t>
-  </si>
-  <si>
-    <t>preproduser@yopmail.com</t>
-  </si>
-  <si>
-    <t>StateTenant</t>
-  </si>
-  <si>
-    <t>suborgdiffbookcreator@yopmail.com</t>
-  </si>
-  <si>
-    <t>SubOrgReviewer</t>
-  </si>
-  <si>
-    <t>suborgdiffcontentreviewer@yopmail.com</t>
-  </si>
-  <si>
-    <t>CreatorRJ</t>
-  </si>
-  <si>
-    <t>contentcreatorRJ@yopmail.com</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>Admin4</t>
-  </si>
-  <si>
-    <t>portalpreprod30@yopmail.com</t>
-  </si>
-  <si>
-    <t>Custod2</t>
-  </si>
-  <si>
-    <t>custod2user@yopmail.com</t>
-  </si>
-  <si>
-    <t>Admin3</t>
-  </si>
-  <si>
-    <t>demoorgadmin@tn.com</t>
-  </si>
-  <si>
-    <t>demo123</t>
-  </si>
-  <si>
-    <t>InvalidUser</t>
-  </si>
-  <si>
-    <t>InvalidUser@yopmail.com</t>
-  </si>
-  <si>
-    <t>Custodian3</t>
-  </si>
-  <si>
-    <t>custodian993@yopmail.com</t>
-  </si>
-  <si>
-    <t>ContentCreator</t>
-  </si>
-  <si>
-    <t>NoBoard</t>
-  </si>
-  <si>
-    <t>bcontentcreator@yopmail.com</t>
-  </si>
-  <si>
-    <t>ContentReviewer</t>
-  </si>
-  <si>
-    <t>contentreviewerTN@yopmail.com</t>
-  </si>
-  <si>
-    <t>ML</t>
-  </si>
-  <si>
-    <t>pnr15@yopmail.com</t>
-  </si>
-  <si>
-    <t>MinorUser</t>
-  </si>
-  <si>
-    <t>childuser@yopmail.com</t>
-  </si>
-  <si>
-    <t>NCERTCC</t>
-  </si>
-  <si>
-    <t>ncertcontentcreator100@yopmail.com</t>
-  </si>
-  <si>
-    <t>Password@123</t>
-  </si>
-  <si>
-    <t>NCERTCR</t>
-  </si>
-  <si>
-    <t>ncertcontentreviewer100@yopmail.com</t>
-  </si>
-  <si>
-    <t>NewCustUser</t>
-  </si>
-  <si>
-    <t>preprod40@yopmail.com</t>
-  </si>
-  <si>
-    <t>VerifyMembers</t>
-  </si>
-  <si>
-    <t>stag58@yopmail.com</t>
-  </si>
-  <si>
-    <t>DeleteGroup1</t>
-  </si>
-  <si>
-    <t>preprod38@yopmail.com</t>
-  </si>
-  <si>
-    <t>deleteMember1</t>
-  </si>
-  <si>
-    <t>group19@yopmail.com</t>
-  </si>
-  <si>
-    <t>Tntenant</t>
-  </si>
-  <si>
-    <t>Tnorgadmin@yopmail.com</t>
-  </si>
-  <si>
-    <t>Admin2</t>
-  </si>
-  <si>
-    <t>APTenantCreator</t>
-  </si>
-  <si>
-    <t>apcontentcreator100@yopmail.com</t>
-  </si>
-  <si>
-    <t>apcontentreviewer100@yopmail.com</t>
-  </si>
-  <si>
-    <t>NewCredCourseToc</t>
-  </si>
-  <si>
-    <t>stag55@yopmail.com</t>
-  </si>
-  <si>
-    <t>Dont Use</t>
-  </si>
-  <si>
-    <t>stagdu@yopmail.com</t>
-  </si>
-  <si>
-    <t>No Groups</t>
-  </si>
-  <si>
-    <t>stagn@yopmail.com</t>
-  </si>
-  <si>
-    <t>Group Member</t>
-  </si>
-  <si>
-    <t>userv1@yopmail.com</t>
-  </si>
-  <si>
-    <t>AddUserCred</t>
-  </si>
-  <si>
-    <t>adduserswitch1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Notification</t>
-  </si>
-  <si>
-    <t>preprod50@yopmail.com</t>
-  </si>
-  <si>
-    <t>submitDetails</t>
-  </si>
-  <si>
-    <t>submitdetailsprofpage@yopmail.com</t>
-  </si>
-  <si>
-    <t>memberaddedgroup</t>
-  </si>
-  <si>
-    <t>memberaddedgroup@yopmail.com</t>
-  </si>
-  <si>
-    <t>MobileNumberRegistedUser</t>
-  </si>
-  <si>
-    <t>certficateTabValidation</t>
-  </si>
-  <si>
-    <t>userdd@yopmail.com</t>
-  </si>
-  <si>
-    <t>ContentCreator1</t>
-  </si>
-  <si>
-    <t>globe1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Pass@123</t>
-  </si>
-  <si>
-    <t>globe</t>
-  </si>
-  <si>
-    <t>CourseName</t>
-  </si>
-  <si>
-    <t>CourseDescription</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>TitleDescription</t>
-  </si>
-  <si>
-    <t>CourseA</t>
-  </si>
-  <si>
-    <t>CourseA Description</t>
-  </si>
-  <si>
-    <t>CourseA Title</t>
-  </si>
-  <si>
-    <t>CourseA Title Description</t>
-  </si>
-  <si>
     <t>CourseB</t>
   </si>
   <si>
@@ -727,12 +754,18 @@
     <t>State (Tamil Nadu)</t>
   </si>
   <si>
+    <t>do_2137393696749649921630</t>
+  </si>
+  <si>
     <t>do_21338107366820249611</t>
   </si>
   <si>
     <t>do_2131551227510784001296</t>
   </si>
   <si>
+    <t>do_31254754341063884829353</t>
+  </si>
+  <si>
     <t>do_213321595703738368112</t>
   </si>
   <si>
@@ -781,6 +814,9 @@
     <t>do_2135757023793479681777</t>
   </si>
   <si>
+    <t>do_2134552729804881921552</t>
+  </si>
+  <si>
     <t>New_Feature_publish</t>
   </si>
   <si>
@@ -892,82 +928,181 @@
     <t>do_213688806051889152117</t>
   </si>
   <si>
+    <t>do_2137096764852387841173</t>
+  </si>
+  <si>
+    <t>do_2135932674933145601746</t>
+  </si>
+  <si>
     <t>do_213688806560997376120</t>
   </si>
   <si>
+    <t>do_2137096755350650881170</t>
+  </si>
+  <si>
     <t>do_213688807068565504123</t>
   </si>
   <si>
+    <t>do_2137096779583242241176</t>
+  </si>
+  <si>
     <t>do_213688807616905216126</t>
   </si>
   <si>
+    <t>Certificate Course</t>
+  </si>
+  <si>
+    <t>do_2134596971107532801138</t>
+  </si>
+  <si>
     <t>do_213688808191664128129</t>
   </si>
   <si>
-    <t>do_2135932674933145601746</t>
-  </si>
-  <si>
-    <t>do_2137096764852387841173</t>
-  </si>
-  <si>
-    <t>do_2137096755350650881170</t>
-  </si>
-  <si>
-    <t>do_2137096779583242241176</t>
-  </si>
-  <si>
-    <t>do_2134596971107532801138</t>
-  </si>
-  <si>
-    <t>OrgAdmin</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>do_2134552729804881921552</t>
-  </si>
-  <si>
-    <t>Certificate Course</t>
-  </si>
-  <si>
-    <t>do_2137393696749649921630</t>
-  </si>
-  <si>
-    <t>submitProfile</t>
-  </si>
-  <si>
-    <t>OnlyCreator</t>
-  </si>
-  <si>
-    <t>do_31254754341063884829353</t>
-  </si>
-  <si>
-    <t>Content Type</t>
-  </si>
-  <si>
-    <t>do_id</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
-    <t>frGdlx</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PDF_Sample_GEOQsm</t>
-  </si>
-  <si>
-    <t>PDF_Sample_CjmniN</t>
-  </si>
-  <si>
-    <t>PDF_Sample_aXZfBn</t>
-  </si>
-  <si>
-    <t>PDF_Sample_LwgwbL</t>
+    <t>PDF_Sample_JabgRG</t>
+  </si>
+  <si>
+    <t>sceaUjmC</t>
+  </si>
+  <si>
+    <t>do_213797848548270080165</t>
+  </si>
+  <si>
+    <t>PDF_Sample_jgQBii</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>CourseHcAXYWua</t>
+  </si>
+  <si>
+    <t>do_213797858137423872169</t>
+  </si>
+  <si>
+    <t>PDF_ContentjiLcxU</t>
+  </si>
+  <si>
+    <t>PDF_ContentcdBTIt</t>
+  </si>
+  <si>
+    <t>PDF_ContentDcaMlx</t>
+  </si>
+  <si>
+    <t>PDF_ContentCHIMSY</t>
+  </si>
+  <si>
+    <t>Course_EEQPDy</t>
+  </si>
+  <si>
+    <t>do_213798480874291200188</t>
+  </si>
+  <si>
+    <t>PDF_ContentqcGEoO</t>
+  </si>
+  <si>
+    <t>Course_XjiKTb</t>
+  </si>
+  <si>
+    <t>do_213798492200001536192</t>
+  </si>
+  <si>
+    <t>PDF_ContentYEGKEX</t>
+  </si>
+  <si>
+    <t>Course_hBhJgT</t>
+  </si>
+  <si>
+    <t>do_2137985473121730561115</t>
+  </si>
+  <si>
+    <t>PDF_ContentgrJOlj</t>
+  </si>
+  <si>
+    <t>Course_ARFpda</t>
+  </si>
+  <si>
+    <t>do_2137985526400122881121</t>
+  </si>
+  <si>
+    <t>PDF_ContentZRfpzx</t>
+  </si>
+  <si>
+    <t>Course_yAAcrF</t>
+  </si>
+  <si>
+    <t>do_2137985819633500161128</t>
+  </si>
+  <si>
+    <t>PDF_ContentwPsmes</t>
+  </si>
+  <si>
+    <t>Course_AYkxcO</t>
+  </si>
+  <si>
+    <t>do_2137991841317109761149</t>
+  </si>
+  <si>
+    <t>PDF_ContentpRmsQO</t>
+  </si>
+  <si>
+    <t>Course_vwQsgQ</t>
+  </si>
+  <si>
+    <t>do_2137992655592570881155</t>
+  </si>
+  <si>
+    <t>PDF_ContenttFRxsr</t>
+  </si>
+  <si>
+    <t>Course_twEmzN</t>
+  </si>
+  <si>
+    <t>do_2137993503546163201164</t>
+  </si>
+  <si>
+    <t>PDF_ContentnqDNLI</t>
+  </si>
+  <si>
+    <t>Course_xViyae</t>
+  </si>
+  <si>
+    <t>do_2137993681980702721172</t>
+  </si>
+  <si>
+    <t>PDF_ContentYYqzpO</t>
+  </si>
+  <si>
+    <t>Course_hYRVtl</t>
+  </si>
+  <si>
+    <t>do_2137993768005632001176</t>
+  </si>
+  <si>
+    <t>PDF_ContentyDoyAf</t>
+  </si>
+  <si>
+    <t>Course_TjWwht</t>
+  </si>
+  <si>
+    <t>do_2137994083620044801212</t>
+  </si>
+  <si>
+    <t>PDF_ContentyCBhsw</t>
+  </si>
+  <si>
+    <t>Course_pjWKIq</t>
+  </si>
+  <si>
+    <t>do_2137994353818255361218</t>
+  </si>
+  <si>
+    <t>PDF_ContentzrrdfQ</t>
+  </si>
+  <si>
+    <t>Course_jvzFKT</t>
+  </si>
+  <si>
+    <t>do_2138013889827471361236</t>
   </si>
 </sst>
 </file>
@@ -978,7 +1113,7 @@
     <numFmt numFmtId="164" formatCode="dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1651,661 +1786,661 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="33.26953125"/>
-    <col min="2" max="2" customWidth="true" style="1" width="42.1796875"/>
+    <col min="1" max="1" customWidth="true" style="1" width="33.28515625"/>
+    <col min="2" max="2" customWidth="true" style="1" width="42.140625"/>
     <col min="3" max="3" customWidth="true" style="1" width="14.0"/>
-    <col min="4" max="16384" style="1" width="10.54296875"/>
+    <col min="4" max="16384" style="1" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.45">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
+      <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="C24" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1">
+      <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="10" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1">
+      <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1">
+      <c r="A29" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="C30" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1">
+      <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="C31" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1">
+      <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1">
+      <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1">
+      <c r="A34" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1">
+      <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1">
+      <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1">
+      <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1">
+      <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="C38" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1">
+      <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="C39" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" customHeight="1">
+      <c r="A40" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1">
+      <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13" t="s">
+      <c r="B41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1">
+      <c r="A42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="C42" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1">
+      <c r="A43" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="15" t="s">
+      <c r="B43" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
+      <c r="C43" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1">
+      <c r="A44" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
+      <c r="C44" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1">
+      <c r="A45" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B45" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16" t="s">
+      <c r="C45" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1">
+      <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" customHeight="1">
+      <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="C47" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" customHeight="1">
+      <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B48" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="C48" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" customHeight="1">
+      <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B49" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="C49" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1">
+      <c r="A50" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+      <c r="C50" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1">
+      <c r="A51" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="B51" s="3">
         <v>9738611076</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1">
       <c r="A52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1">
+      <c r="A53" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="3" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1">
+      <c r="A54" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="B54" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1">
+      <c r="A55" s="28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="14" t="s">
+      <c r="B55" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" customHeight="1">
+      <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="B55" s="29" t="s">
+      <c r="B56" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>16</v>
-      </c>
       <c r="C56" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1">
       <c r="A58" s="30" t="s">
-        <v>299</v>
+        <v>108</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1">
       <c r="A59" s="30" t="s">
-        <v>300</v>
+        <v>109</v>
       </c>
       <c r="B59" s="33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2380,91 +2515,410 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37638-8D6C-48B3-B1A2-643F9FBAF64C}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.08984375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="4.453125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.54296875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.26953125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.5703125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.45">
       <c r="A1" s="2" t="s">
-        <v>302</v>
+        <v>110</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>303</v>
+        <v>112</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>306</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>307</v>
       </c>
       <c r="C3" t="s">
-        <v>306</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>308</v>
       </c>
       <c r="C4" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C5" t="s">
-        <v>306</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C6" t="s">
-        <v>306</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>323</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>326</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" t="s">
+        <v>327</v>
+      </c>
+      <c r="C17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>329</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" t="s">
+        <v>332</v>
+      </c>
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>335</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" t="s">
+        <v>336</v>
+      </c>
+      <c r="C23" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>338</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>311</v>
+      </c>
+      <c r="B25" t="s">
+        <v>339</v>
+      </c>
+      <c r="C25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C27" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>344</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29" t="s">
+        <v>345</v>
+      </c>
+      <c r="C29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>347</v>
+      </c>
+      <c r="C30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>311</v>
+      </c>
+      <c r="B31" t="s">
+        <v>348</v>
+      </c>
+      <c r="C31" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>350</v>
+      </c>
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B33" t="s">
+        <v>351</v>
+      </c>
+      <c r="C33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>353</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>311</v>
+      </c>
+      <c r="B35" t="s">
+        <v>354</v>
+      </c>
+      <c r="C35" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -2480,1215 +2934,1215 @@
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="43.453125"/>
-    <col min="2" max="2" customWidth="true" style="3" width="29.54296875"/>
-    <col min="3" max="3" customWidth="true" style="3" width="34.54296875"/>
-    <col min="4" max="4" customWidth="true" style="3" width="29.54296875"/>
-    <col min="5" max="5" customWidth="true" style="3" width="16.54296875"/>
-    <col min="6" max="16384" style="3" width="10.54296875"/>
+    <col min="1" max="1" customWidth="true" style="3" width="43.42578125"/>
+    <col min="2" max="2" customWidth="true" style="3" width="29.5703125"/>
+    <col min="3" max="3" customWidth="true" style="3" width="34.5703125"/>
+    <col min="4" max="4" customWidth="true" style="3" width="29.5703125"/>
+    <col min="5" max="5" customWidth="true" style="3" width="16.5703125"/>
+    <col min="6" max="16384" style="3" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F8" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F9" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="C10" s="19">
         <f ca="1">TODAY()</f>
-        <v>45061</v>
+        <v>45062</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F10" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F11" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="45" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F12" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F13" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F14" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F15" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F16" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F17" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F18" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F19" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F20" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F21" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F22" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="21" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F23" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F24" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F25" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F26" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F27" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F28" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F29" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F30" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F31" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F32" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F33" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C34" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F34" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="21" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F35" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F36" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="23" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F37" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F38" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F39" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="21" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>301</v>
+        <v>242</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="F40" s="3">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="13" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="F41" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="D42" s="3" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F42" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F43" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="B44" s="3" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F44" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F45" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="B46" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F46" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F47" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F48" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F49" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F50" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="C51" s="3" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F51" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F52" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="B53" s="3" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D53" s="16">
         <v>33291500301</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F53" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F54" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F55" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F56" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="15" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F57" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15" customHeight="1">
       <c r="A58" s="25" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F58" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="15" customHeight="1">
       <c r="A59" s="26">
         <f ca="1">TODAY()+1</f>
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F59" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="15" customHeight="1">
       <c r="A60" s="26">
         <f ca="1">TODAY()+2</f>
-        <v>45063</v>
+        <v>45064</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F60" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="15" customHeight="1">
       <c r="A61" s="26">
         <f ca="1">TODAY()+3</f>
-        <v>45064</v>
+        <v>45065</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F61" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="15" customHeight="1">
       <c r="A62" s="26">
         <f ca="1">TODAY()+4</f>
-        <v>45065</v>
+        <v>45066</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F62" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="26">
         <f ca="1">A60</f>
-        <v>45063</v>
+        <v>45064</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F63" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F64" s="3">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F65" s="3">
         <v>63</v>

</xml_diff>